<commit_message>
Final runs + batch for instsance57 full runs
</commit_message>
<xml_diff>
--- a/analysis/02-10-2018 - tmp - table4michal.xlsx
+++ b/analysis/02-10-2018 - tmp - table4michal.xlsx
@@ -103,7 +103,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +123,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
       </patternFill>
     </fill>
   </fills>
@@ -150,14 +155,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -187,11 +193,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
+    <cellStyle name="Accent4" xfId="5" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -489,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -522,11 +532,11 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">

</xml_diff>